<commit_message>
Minor edits to template
</commit_message>
<xml_diff>
--- a/data/tiltaksovervakingen_blank_data_template.xlsx
+++ b/data/tiltaksovervakingen_blank_data_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1B2770-4A07-47CF-A68A-9BA801C221C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B1F858-6E8A-4C3C-9860-0BDFCA072EE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,9 +138,6 @@
     <t>mg/l</t>
   </si>
   <si>
-    <t>Analyseresultater fra forsurede og kalkede vassdrag - kvartalsrapport nr. 1 / årsrapport 2022</t>
-  </si>
-  <si>
     <t>Lokalitets-ID</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>Resultatkommentar</t>
+  </si>
+  <si>
+    <t>Analyseresultater fra forsurede og kalkede vassdrag - kvartalsrapport nr. XXX / årsrapport XXXX</t>
   </si>
 </sst>
 </file>
@@ -649,7 +649,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" sqref="A1:AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -680,7 +680,7 @@
   <sheetData>
     <row r="1" spans="1:30" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>2</v>
@@ -872,10 +872,10 @@
         <v>32</v>
       </c>
       <c r="AC3" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD3" s="22" t="s">
         <v>37</v>
-      </c>
-      <c r="AD3" s="22" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add date validation to template
</commit_message>
<xml_diff>
--- a/data/tiltaksovervakingen_blank_data_template.xlsx
+++ b/data/tiltaksovervakingen_blank_data_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Oeyvind_G\Tiltaksovervakingen\tiltaksovervakingen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B1F858-6E8A-4C3C-9860-0BDFCA072EE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB15F3E-AC8E-4521-8395-01C1A5EAAD21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -240,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -307,6 +307,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,11 +646,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AD14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:AD1"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -878,6 +879,9 @@
         <v>37</v>
       </c>
     </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="G14" s="24"/>
+    </row>
   </sheetData>
   <autoFilter ref="A3:AD3" xr:uid="{1A4FF15F-C237-4D80-81AB-70C3E753FD43}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:AL3">
@@ -889,6 +893,12 @@
   <mergeCells count="1">
     <mergeCell ref="A1:AD1"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Date error" error="Please enter a date." sqref="G1:G1048576" xr:uid="{B3A9CFDE-4BF7-49A1-8D92-23B1DFC7C912}">
+      <formula1>40179</formula1>
+      <formula2>47484</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>